<commit_message>
Data analytics with python
</commit_message>
<xml_diff>
--- a/Data analytics with python/PROBLEM 1.xlsx
+++ b/Data analytics with python/PROBLEM 1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="176">
   <si>
     <t>TASK ID</t>
   </si>
@@ -119,6 +119,9 @@
     <t>MS0001</t>
   </si>
   <si>
+    <t>31/11/2021</t>
+  </si>
+  <si>
     <t>Giridhar Yerra</t>
   </si>
   <si>
@@ -543,6 +546,9 @@
   </si>
   <si>
     <t>DB00002</t>
+  </si>
+  <si>
+    <t>23/10/2021</t>
   </si>
   <si>
     <t>VS2021103102</t>
@@ -988,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D36" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1043,7 +1049,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>11</v>
@@ -1073,7 +1079,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>16</v>
@@ -1103,7 +1109,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>21</v>
@@ -1145,10 +1151,10 @@
         <v>30</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="I5" s="5">
         <v>1</v>
@@ -1157,22 +1163,22 @@
     </row>
     <row r="6" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>14</v>
@@ -1180,29 +1186,29 @@
       <c r="H6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="2">
-        <v>1</v>
-      </c>
-      <c r="J6" s="5"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>19</v>
@@ -1210,35 +1216,35 @@
       <c r="H7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="2">
-        <v>1</v>
-      </c>
-      <c r="J7" s="5"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I8" s="2">
         <v>1</v>
@@ -1247,112 +1253,112 @@
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="5">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1</v>
-      </c>
-      <c r="J10" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="2">
-        <v>1</v>
-      </c>
-      <c r="J11" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>14</v>
@@ -1367,112 +1373,112 @@
     </row>
     <row r="13" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="5">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="5">
-        <v>1</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="5">
-        <v>1</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>14</v>
@@ -1487,22 +1493,22 @@
     </row>
     <row r="17" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>19</v>
@@ -1517,22 +1523,22 @@
     </row>
     <row r="18" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>24</v>
@@ -1547,28 +1553,28 @@
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I19" s="2">
         <v>1</v>
@@ -1577,28 +1583,28 @@
     </row>
     <row r="20" spans="1:10" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I20" s="2">
         <v>1</v>
@@ -1607,22 +1613,22 @@
     </row>
     <row r="21" spans="1:10" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>25</v>
@@ -1637,28 +1643,28 @@
     </row>
     <row r="22" spans="1:10" ht="56.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I22" s="2">
         <v>1</v>
@@ -1667,22 +1673,22 @@
     </row>
     <row r="23" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>14</v>
@@ -1697,22 +1703,22 @@
     </row>
     <row r="24" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>19</v>
@@ -1727,22 +1733,22 @@
     </row>
     <row r="25" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>24</v>
@@ -1757,28 +1763,28 @@
     </row>
     <row r="26" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I26" s="2">
         <v>1</v>
@@ -1787,28 +1793,28 @@
     </row>
     <row r="27" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I27" s="2">
         <v>1</v>
@@ -1817,22 +1823,22 @@
     </row>
     <row r="28" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>25</v>
@@ -1847,28 +1853,28 @@
     </row>
     <row r="29" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I29" s="2">
         <v>1</v>
@@ -1877,28 +1883,28 @@
     </row>
     <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I30" s="2">
         <v>1</v>
@@ -1907,25 +1913,25 @@
     </row>
     <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>25</v>
@@ -1937,28 +1943,28 @@
     </row>
     <row r="32" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2">
@@ -1967,22 +1973,22 @@
     </row>
     <row r="33" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>14</v>
@@ -1997,22 +2003,22 @@
     </row>
     <row r="34" spans="1:10" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="D34" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>19</v>
@@ -2027,22 +2033,22 @@
     </row>
     <row r="35" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="D35" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>24</v>
@@ -2057,28 +2063,28 @@
     </row>
     <row r="36" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="D36" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I36" s="2">
         <v>1</v>
@@ -2087,28 +2093,28 @@
     </row>
     <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>160</v>
-      </c>
       <c r="E37" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I37" s="2">
         <v>1</v>
@@ -2117,13 +2123,13 @@
     </row>
     <row r="38" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>12</v>
@@ -2147,13 +2153,13 @@
     </row>
     <row r="39" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>17</v>
@@ -2165,10 +2171,10 @@
         <v>18</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I39" s="2">
         <v>1</v>
@@ -2177,25 +2183,25 @@
     </row>
     <row r="40" spans="1:10" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>14</v>
+        <v>174</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>14</v>
@@ -2207,28 +2213,28 @@
     </row>
     <row r="41" spans="1:10" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I41" s="2">
         <v>1</v>
@@ -2237,28 +2243,28 @@
     </row>
     <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H42" s="8" t="s">
-        <v>25</v>
+      <c r="H42" s="8">
+        <v>44266</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2">
@@ -2267,28 +2273,28 @@
     </row>
     <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="H43" s="8">
+        <v>44238</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2">

</xml_diff>